<commit_message>
Fix a couple issues with csvs and mexs
</commit_message>
<xml_diff>
--- a/data/coded_segments/bw_1_1.xlsx
+++ b/data/coded_segments/bw_1_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1954352E-534B-9249-97CD-7F405726D108}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EEBC408-D26E-514D-AEF9-1BD69DFBC443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2260" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAXQDA 12" sheetId="1" r:id="rId1"/>
@@ -4932,16 +4932,19 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF909090"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -5384,9 +5387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
More fixes to mex files and update QA checks in index_articles
</commit_message>
<xml_diff>
--- a/data/coded_segments/bw_1_1.xlsx
+++ b/data/coded_segments/bw_1_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EEBC408-D26E-514D-AEF9-1BD69DFBC443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4658A74A-2B0E-274F-A928-7A84D9B0B169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAXQDA 12" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5763" uniqueCount="1534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5853" uniqueCount="1567">
   <si>
     <t>Color</t>
   </si>
@@ -4918,6 +4918,105 @@
   </si>
   <si>
     <t>08/14/2019 13:40:51</t>
+  </si>
+  <si>
+    <t>16897</t>
+  </si>
+  <si>
+    <t>1: 2832</t>
+  </si>
+  <si>
+    <t>1: 2833</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:29:14</t>
+  </si>
+  <si>
+    <t>1: 2844</t>
+  </si>
+  <si>
+    <t>1: 2847</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:29:21</t>
+  </si>
+  <si>
+    <t>1: 2850</t>
+  </si>
+  <si>
+    <t>1: 2857</t>
+  </si>
+  <si>
+    <t>diabetic</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:29:29</t>
+  </si>
+  <si>
+    <t>1: 146</t>
+  </si>
+  <si>
+    <t>1: 164</t>
+  </si>
+  <si>
+    <t>Nocardia asteroides</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:30:29</t>
+  </si>
+  <si>
+    <t>1: 3552</t>
+  </si>
+  <si>
+    <t>1: 3555</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:30:48</t>
+  </si>
+  <si>
+    <t>1: 3557</t>
+  </si>
+  <si>
+    <t>1: 3560</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:30:52</t>
+  </si>
+  <si>
+    <t>1: 5495</t>
+  </si>
+  <si>
+    <t>1: 5523</t>
+  </si>
+  <si>
+    <t>trimethoprim–sulfamethoxazole</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:31:56</t>
+  </si>
+  <si>
+    <t>1: 6298</t>
+  </si>
+  <si>
+    <t>1: 6301</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:33:26</t>
+  </si>
+  <si>
+    <t>1: 3235</t>
+  </si>
+  <si>
+    <t>1: 3239</t>
+  </si>
+  <si>
+    <t>08/21/2019 15:36:26</t>
   </si>
 </sst>
 </file>
@@ -5385,7 +5484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M576"/>
+  <dimension ref="A1:M585"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29017,6 +29116,375 @@
         <v>1533</v>
       </c>
     </row>
+    <row r="577" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A577" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B577" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C577" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D577" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E577" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F577" s="1" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G577" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="H577" s="3">
+        <v>0</v>
+      </c>
+      <c r="I577" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="J577" s="3">
+        <v>2</v>
+      </c>
+      <c r="K577" s="4">
+        <v>1.3185654008438817E-2</v>
+      </c>
+      <c r="L577" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M577" s="1" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="578" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A578" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B578" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C578" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D578" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E578" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F578" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G578" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="H578" s="3">
+        <v>0</v>
+      </c>
+      <c r="I578" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="J578" s="3">
+        <v>4</v>
+      </c>
+      <c r="K578" s="4">
+        <v>2.6371308016877634E-2</v>
+      </c>
+      <c r="L578" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M578" s="1" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="579" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A579" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B579" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D579" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E579" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F579" s="1" t="s">
+        <v>1543</v>
+      </c>
+      <c r="G579" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="H579" s="3">
+        <v>0</v>
+      </c>
+      <c r="I579" s="2" t="s">
+        <v>1545</v>
+      </c>
+      <c r="J579" s="3">
+        <v>8</v>
+      </c>
+      <c r="K579" s="4">
+        <v>5.2742616033755269E-2</v>
+      </c>
+      <c r="L579" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M579" s="1" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="580" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A580" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B580" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C580" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D580" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E580" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F580" s="1" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G580" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="H580" s="3">
+        <v>0</v>
+      </c>
+      <c r="I580" s="2" t="s">
+        <v>1549</v>
+      </c>
+      <c r="J580" s="3">
+        <v>19</v>
+      </c>
+      <c r="K580" s="4">
+        <v>0.12526371308016879</v>
+      </c>
+      <c r="L580" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M580" s="1" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="581" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A581" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B581" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C581" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D581" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E581" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="F581" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="G581" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="H581" s="3">
+        <v>0</v>
+      </c>
+      <c r="I581" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="J581" s="3">
+        <v>4</v>
+      </c>
+      <c r="K581" s="4">
+        <v>2.6371308016877634E-2</v>
+      </c>
+      <c r="L581" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M581" s="1" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="582" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A582" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B582" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D582" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E582" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F582" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="G582" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="H582" s="3">
+        <v>0</v>
+      </c>
+      <c r="I582" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="J582" s="3">
+        <v>4</v>
+      </c>
+      <c r="K582" s="4">
+        <v>2.6371308016877634E-2</v>
+      </c>
+      <c r="L582" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M582" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="583" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A583" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B583" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C583" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D583" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E583" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F583" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="G583" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="H583" s="3">
+        <v>0</v>
+      </c>
+      <c r="I583" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="J583" s="3">
+        <v>29</v>
+      </c>
+      <c r="K583" s="4">
+        <v>0.19119198312236288</v>
+      </c>
+      <c r="L583" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M583" s="1" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="584" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A584" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B584" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C584" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D584" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E584" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="F584" s="1" t="s">
+        <v>1561</v>
+      </c>
+      <c r="G584" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="H584" s="3">
+        <v>0</v>
+      </c>
+      <c r="I584" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="J584" s="3">
+        <v>4</v>
+      </c>
+      <c r="K584" s="4">
+        <v>2.6371308016877634E-2</v>
+      </c>
+      <c r="L584" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M584" s="1" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="585" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A585" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B585" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C585" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D585" s="2" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E585" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F585" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="G585" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="H585" s="3">
+        <v>0</v>
+      </c>
+      <c r="I585" s="2" t="s">
+        <v>947</v>
+      </c>
+      <c r="J585" s="3">
+        <v>5</v>
+      </c>
+      <c r="K585" s="4">
+        <v>3.2964135021097046E-2</v>
+      </c>
+      <c r="L585" s="1" t="s">
+        <v>1538</v>
+      </c>
+      <c r="M585" s="1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>